<commit_message>
pdf version of schedule
</commit_message>
<xml_diff>
--- a/CIS355FALL2014schedule.xlsx
+++ b/CIS355FALL2014schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwclark2\Dropbox\Teaching\CIS355\FALL2014\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwclark2\Dropbox\Teaching\CIS355\course-info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
   <si>
     <t>topic</t>
   </si>
@@ -102,9 +102,6 @@
     <t>prof notes</t>
   </si>
   <si>
-    <t>teal = not finalized</t>
-  </si>
-  <si>
     <t>grade part</t>
   </si>
   <si>
@@ -150,15 +147,6 @@
     <t>database hack day</t>
   </si>
   <si>
-    <t>intro to databases + PostgreSQL hack day</t>
-  </si>
-  <si>
-    <t>install PostgreSQL and bring laptop</t>
-  </si>
-  <si>
-    <t>intro to databases and then fire up PostgreSQL</t>
-  </si>
-  <si>
     <t>conceptual diagram</t>
   </si>
   <si>
@@ -267,19 +255,12 @@
     <t>guest speaker here would be ideal</t>
   </si>
   <si>
-    <t>guest speaker on agile DW/BI here?</t>
-  </si>
-  <si>
     <t>BI at Guthy-Renker (file)</t>
   </si>
   <si>
     <t>git, github, and the CIS 355 project</t>
   </si>
   <si>
-    <t>try.github.io , tinyurl.com/39hd87l ,
-Kimball + Ross TOC, introduction</t>
-  </si>
-  <si>
     <t>project repo setup + README</t>
   </si>
   <si>
@@ -334,7 +315,28 @@
     <t>Arizona Tech Summit is today, 8am-5pm</t>
   </si>
   <si>
-    <t>midterm exam -- proctored if I'm out of town</t>
+    <t>the big picture</t>
+  </si>
+  <si>
+    <t>Kimball + Ross TOC, introduction</t>
+  </si>
+  <si>
+    <t>try.github.io , tinyurl.com/39hd87l</t>
+  </si>
+  <si>
+    <t>fire up PostgreSQL and create tables, add data</t>
+  </si>
+  <si>
+    <t>show how to "dump" database schema to version control</t>
+  </si>
+  <si>
+    <t>define assignments by this point</t>
+  </si>
+  <si>
+    <t>midterm exam</t>
+  </si>
+  <si>
+    <t>PROF OUT OF TOWN - video lecture</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1184,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,13 +1203,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1"/>
       <c r="E1" s="43"/>
       <c r="F1" s="44">
         <f ca="1">TODAY()</f>
-        <v>41872</v>
+        <v>41873</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1216,9 +1218,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="37" t="s">
-        <v>26</v>
-      </c>
+      <c r="D2" s="37"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1247,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1258,32 +1258,32 @@
         <v>41876</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="E4" s="14"/>
-      <c r="F4" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="19">
         <v>41878</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D5" s="67" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>41883</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="53"/>
       <c r="E6" s="48"/>
@@ -1308,14 +1308,17 @@
         <v>41885</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="13" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I7" s="41">
         <v>5</v>
@@ -1330,15 +1333,15 @@
         <v>41890</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="54"/>
       <c r="E8" s="16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F8" s="10"/>
       <c r="H8" s="41" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="I8" s="41">
         <v>5</v>
@@ -1351,10 +1354,13 @@
         <v>41892</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="55"/>
       <c r="E9" s="13"/>
+      <c r="F9" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -1365,17 +1371,17 @@
         <v>41897</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I10" s="41">
         <v>5</v>
@@ -1388,12 +1394,12 @@
         <v>41899</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="13"/>
       <c r="F11" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1405,20 +1411,20 @@
         <v>41904</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I12" s="41">
         <v>5</v>
@@ -1431,10 +1437,10 @@
         <v>41906</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="52" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="9"/>
@@ -1448,10 +1454,10 @@
         <v>41911</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="9"/>
@@ -1463,14 +1469,14 @@
         <v>41913</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="55"/>
       <c r="E15" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I15" s="40">
         <v>5</v>
@@ -1485,12 +1491,12 @@
         <v>41918</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="14"/>
       <c r="F16" s="66" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1500,7 +1506,7 @@
         <v>41920</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="13"/>
@@ -1520,10 +1526,10 @@
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="I18" s="41">
         <v>5</v>
@@ -1541,10 +1547,10 @@
       <c r="D19" s="55"/>
       <c r="E19" s="13"/>
       <c r="F19" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I19" s="40">
         <v>15</v>
@@ -1559,13 +1565,15 @@
         <v>41932</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E20" s="14"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="9" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
@@ -1574,12 +1582,12 @@
         <v>41934</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="47"/>
-      <c r="F21" s="66" t="s">
-        <v>81</v>
+      <c r="F21" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1591,15 +1599,15 @@
         <v>41939</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F22" s="9"/>
       <c r="H22" s="41" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I22" s="41">
         <v>5</v>
@@ -1612,10 +1620,10 @@
         <v>41941</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E23" s="13"/>
     </row>
@@ -1628,7 +1636,7 @@
         <v>41946</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="14"/>
@@ -1641,14 +1649,14 @@
         <v>41948</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1660,17 +1668,17 @@
         <v>41953</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="50" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H26" s="41" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I26" s="41">
         <v>5</v>
@@ -1683,12 +1691,12 @@
         <v>41955</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D27" s="55"/>
       <c r="E27" s="13"/>
       <c r="F27" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1700,14 +1708,14 @@
         <v>41960</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="66" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1717,7 +1725,7 @@
         <v>41962</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D29" s="52"/>
       <c r="E29" s="13"/>
@@ -1731,16 +1739,16 @@
         <v>41967</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D30" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="60" t="s">
-        <v>71</v>
-      </c>
       <c r="H30" s="41" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="I30" s="41">
         <v>5</v>
@@ -1753,12 +1761,12 @@
         <v>41969</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="58"/>
       <c r="F31" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1770,10 +1778,10 @@
         <v>41974</v>
       </c>
       <c r="C32" s="60" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E32" s="38"/>
     </row>
@@ -1784,15 +1792,15 @@
         <v>41976</v>
       </c>
       <c r="C33" s="65" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D33" s="55"/>
       <c r="E33" s="33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F33" s="11"/>
       <c r="H33" s="41" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I33" s="41">
         <v>10</v>
@@ -1807,14 +1815,14 @@
         <v>41981</v>
       </c>
       <c r="C34" s="64" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H34" s="40" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I34" s="40">
         <v>20</v>
@@ -1830,7 +1838,7 @@
       <c r="D35" s="29"/>
       <c r="E35" s="17"/>
       <c r="H35" s="42" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I35" s="42">
         <v>10</v>
@@ -1841,11 +1849,11 @@
       <c r="B36" s="32"/>
       <c r="C36" s="32"/>
       <c r="D36" s="45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E36" s="46">
         <f ca="1">TODAY()</f>
-        <v>41872</v>
+        <v>41873</v>
       </c>
       <c r="I36" s="8">
         <f>SUM(I4:I35)</f>

</xml_diff>

<commit_message>
moved midterm 1 week later
</commit_message>
<xml_diff>
--- a/CIS355FALL2014schedule.xlsx
+++ b/CIS355FALL2014schedule.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
   <si>
     <t>topic</t>
   </si>
@@ -156,12 +156,6 @@
     <t>K+R chapter 4</t>
   </si>
   <si>
-    <t>Kimball architecture + conformed dimensions</t>
-  </si>
-  <si>
-    <t>inventory hack day</t>
-  </si>
-  <si>
     <t>project requirements - 2nd cut</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>define assignments by this point</t>
   </si>
   <si>
-    <t>midterm exam</t>
-  </si>
-  <si>
     <t>PROF OUT OF TOWN - video lecture</t>
   </si>
   <si>
@@ -334,6 +325,12 @@
   </si>
   <si>
     <t>ER diagram + requirements</t>
+  </si>
+  <si>
+    <t>midterm review: Kimball architecture</t>
+  </si>
+  <si>
+    <t>data on the cloud</t>
   </si>
 </sst>
 </file>
@@ -696,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -873,6 +870,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1212,7 @@
       <c r="E1" s="43"/>
       <c r="F1" s="44">
         <f ca="1">TODAY()</f>
-        <v>41897</v>
+        <v>41918</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1261,10 +1261,10 @@
         <v>41876</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E4" s="14"/>
     </row>
@@ -1274,19 +1274,19 @@
         <v>41878</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="67" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1315,13 +1315,13 @@
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I7" s="41">
         <v>5</v>
@@ -1368,7 +1368,7 @@
       <c r="D10" s="28"/>
       <c r="E10" s="14"/>
       <c r="F10" s="35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1382,13 +1382,13 @@
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I11" s="41">
         <v>5</v>
@@ -1406,17 +1406,17 @@
         <v>33</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I12" s="41">
         <v>5</v>
@@ -1435,11 +1435,11 @@
         <v>39</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F13" s="9"/>
       <c r="H13" s="41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I13" s="41">
         <v>5</v>
@@ -1454,7 +1454,7 @@
         <v>41911</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>40</v>
@@ -1473,10 +1473,10 @@
       </c>
       <c r="D15" s="55"/>
       <c r="E15" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I15" s="40">
         <v>5</v>
@@ -1491,12 +1491,12 @@
         <v>41918</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="14"/>
       <c r="F16" s="66" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1525,11 +1525,11 @@
         <v>19</v>
       </c>
       <c r="D18" s="30"/>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="70" t="s">
         <v>41</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I18" s="41">
         <v>5</v>
@@ -1541,16 +1541,18 @@
         <f t="shared" si="0"/>
         <v>41927</v>
       </c>
-      <c r="C19" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="55"/>
+      <c r="C19" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>43</v>
+      </c>
       <c r="E19" s="13"/>
       <c r="F19" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I19" s="40">
         <v>15</v>
@@ -1565,14 +1567,12 @@
         <v>41932</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>43</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D20" s="28"/>
       <c r="E20" s="14"/>
       <c r="F20" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1581,14 +1581,12 @@
         <f t="shared" si="0"/>
         <v>41934</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>44</v>
+      <c r="C21" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="47"/>
-      <c r="F21" s="9" t="s">
-        <v>93</v>
-      </c>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
@@ -1598,16 +1596,16 @@
         <f t="shared" si="0"/>
         <v>41939</v>
       </c>
-      <c r="C22" s="61" t="s">
-        <v>45</v>
+      <c r="C22" s="60" t="s">
+        <v>102</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F22" s="9"/>
       <c r="H22" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I22" s="41">
         <v>5</v>
@@ -1620,10 +1618,10 @@
         <v>41941</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="13"/>
     </row>
@@ -1636,7 +1634,7 @@
         <v>41946</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="14"/>
@@ -1649,14 +1647,14 @@
         <v>41948</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1668,17 +1666,17 @@
         <v>41953</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H26" s="41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I26" s="41">
         <v>5</v>
@@ -1691,12 +1689,12 @@
         <v>41955</v>
       </c>
       <c r="C27" s="69" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D27" s="55"/>
       <c r="E27" s="13"/>
       <c r="F27" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1708,14 +1706,14 @@
         <v>41960</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="28" t="s">
         <v>52</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>54</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1725,7 +1723,7 @@
         <v>41962</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" s="52"/>
       <c r="E29" s="13"/>
@@ -1739,19 +1737,19 @@
         <v>41967</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30" s="60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I30" s="41">
         <v>5</v>
@@ -1764,12 +1762,12 @@
         <v>41969</v>
       </c>
       <c r="C31" s="68" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="58"/>
       <c r="F31" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1781,10 +1779,10 @@
         <v>41974</v>
       </c>
       <c r="C32" s="60" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E32" s="38"/>
     </row>
@@ -1795,15 +1793,15 @@
         <v>41976</v>
       </c>
       <c r="C33" s="65" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" s="55"/>
       <c r="E33" s="33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F33" s="11"/>
       <c r="H33" s="41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I33" s="41">
         <v>10</v>
@@ -1818,14 +1816,14 @@
         <v>41981</v>
       </c>
       <c r="C34" s="64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H34" s="40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I34" s="40">
         <v>20</v>
@@ -1841,7 +1839,7 @@
       <c r="D35" s="29"/>
       <c r="E35" s="17"/>
       <c r="H35" s="42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I35" s="42">
         <v>10</v>
@@ -1856,7 +1854,7 @@
       </c>
       <c r="E36" s="46">
         <f ca="1">TODAY()</f>
-        <v>41897</v>
+        <v>41918</v>
       </c>
       <c r="I36" s="8">
         <f>SUM(I4:I35)</f>

</xml_diff>

<commit_message>
python script for week 11
</commit_message>
<xml_diff>
--- a/CIS355FALL2014schedule.xlsx
+++ b/CIS355FALL2014schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwclark2\Dropbox\Work\Teaching\CIS355\course-info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Work\Teaching\CIS355\course-info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>topic</t>
   </si>
@@ -159,42 +159,9 @@
     <t>project requirements - 2nd cut</t>
   </si>
   <si>
-    <t>K+R chapter 5</t>
-  </si>
-  <si>
-    <t>procurement - slowly changing dimensions</t>
-  </si>
-  <si>
-    <t>procurement hack day</t>
-  </si>
-  <si>
-    <t>order management</t>
-  </si>
-  <si>
-    <t>order management hack day</t>
-  </si>
-  <si>
-    <t>ETL for professionals</t>
-  </si>
-  <si>
-    <t>K+R chapter 6</t>
-  </si>
-  <si>
-    <t>K+R chapter 19</t>
-  </si>
-  <si>
-    <t>more ETL techniques</t>
-  </si>
-  <si>
-    <t>K+R chapter 20</t>
-  </si>
-  <si>
     <t>big data analytics</t>
   </si>
   <si>
-    <t>K+R chapter 21</t>
-  </si>
-  <si>
     <t>first transforms + deliverables</t>
   </si>
   <si>
@@ -222,9 +189,6 @@
     <t>transactional DB</t>
   </si>
   <si>
-    <t>guest speaker here would be ideal</t>
-  </si>
-  <si>
     <t>BI at Guthy-Renker (file)</t>
   </si>
   <si>
@@ -315,9 +279,6 @@
     <t>NoSQL databases + analytics appliances</t>
   </si>
   <si>
-    <t>Hadoop, MapReduce, Apache Spark</t>
-  </si>
-  <si>
     <t>Chris &amp; Schuyler's honors contract topics</t>
   </si>
   <si>
@@ -330,7 +291,28 @@
     <t>midterm review: Kimball architecture</t>
   </si>
   <si>
-    <t>data on the cloud</t>
+    <t>big data context</t>
+  </si>
+  <si>
+    <t>data infrastructure as a service</t>
+  </si>
+  <si>
+    <t>data formats for communication</t>
+  </si>
+  <si>
+    <t>massivelly parallel processing</t>
+  </si>
+  <si>
+    <t>Apache Spark</t>
+  </si>
+  <si>
+    <t>the elephant in the room: Hadoop</t>
+  </si>
+  <si>
+    <t>data transformation and munging</t>
+  </si>
+  <si>
+    <t>a data web service model</t>
   </si>
 </sst>
 </file>
@@ -693,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -850,9 +832,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,10 +848,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1187,7 +1166,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1191,7 @@
       <c r="E1" s="43"/>
       <c r="F1" s="44">
         <f ca="1">TODAY()</f>
-        <v>41918</v>
+        <v>41939</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1261,10 +1240,10 @@
         <v>41876</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E4" s="14"/>
     </row>
@@ -1274,19 +1253,19 @@
         <v>41878</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="67" t="s">
-        <v>86</v>
+        <v>56</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>74</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1315,13 +1294,13 @@
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="13" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H7" s="41" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="I7" s="41">
         <v>5</v>
@@ -1368,7 +1347,7 @@
       <c r="D10" s="28"/>
       <c r="E10" s="14"/>
       <c r="F10" s="35" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1382,13 +1361,13 @@
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="13" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="I11" s="41">
         <v>5</v>
@@ -1406,17 +1385,17 @@
         <v>33</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="I12" s="41">
         <v>5</v>
@@ -1435,11 +1414,11 @@
         <v>39</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="F13" s="9"/>
       <c r="H13" s="41" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="I13" s="41">
         <v>5</v>
@@ -1454,7 +1433,7 @@
         <v>41911</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>40</v>
@@ -1473,10 +1452,10 @@
       </c>
       <c r="D15" s="55"/>
       <c r="E15" s="13" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="I15" s="40">
         <v>5</v>
@@ -1491,12 +1470,12 @@
         <v>41918</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="66" t="s">
-        <v>82</v>
+      <c r="F16" s="65" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1525,11 +1504,11 @@
         <v>19</v>
       </c>
       <c r="D18" s="30"/>
-      <c r="E18" s="70" t="s">
+      <c r="E18" s="68" t="s">
         <v>41</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="I18" s="41">
         <v>5</v>
@@ -1549,10 +1528,10 @@
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="8" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I19" s="40">
         <v>15</v>
@@ -1567,12 +1546,12 @@
         <v>41932</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="14"/>
       <c r="F20" s="9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1582,7 +1561,7 @@
         <v>41934</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="47"/>
@@ -1597,7 +1576,7 @@
         <v>41939</v>
       </c>
       <c r="C22" s="60" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="14" t="s">
@@ -1605,7 +1584,7 @@
       </c>
       <c r="F22" s="9"/>
       <c r="H22" s="41" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="I22" s="41">
         <v>5</v>
@@ -1618,11 +1597,9 @@
         <v>41941</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="55" t="s">
-        <v>45</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D23" s="55"/>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1633,8 +1610,8 @@
         <f t="shared" si="0"/>
         <v>41946</v>
       </c>
-      <c r="C24" s="62" t="s">
-        <v>47</v>
+      <c r="C24" s="69" t="s">
+        <v>91</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="14"/>
@@ -1647,14 +1624,12 @@
         <v>41948</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="55" t="s">
-        <v>51</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D25" s="55"/>
       <c r="E25" s="13"/>
       <c r="F25" s="35" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1665,18 +1640,18 @@
         <f t="shared" si="0"/>
         <v>41953</v>
       </c>
-      <c r="C26" s="63" t="s">
-        <v>49</v>
+      <c r="C26" s="62" t="s">
+        <v>92</v>
       </c>
       <c r="D26" s="49"/>
       <c r="E26" s="50" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H26" s="41" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="I26" s="41">
         <v>5</v>
@@ -1688,14 +1663,11 @@
         <f t="shared" si="0"/>
         <v>41955</v>
       </c>
-      <c r="C27" s="69" t="s">
-        <v>97</v>
+      <c r="C27" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="D27" s="55"/>
       <c r="E27" s="13"/>
-      <c r="F27" s="8" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="28" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
@@ -1706,14 +1678,12 @@
         <v>41960</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>52</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D28" s="28"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="66" t="s">
-        <v>66</v>
+      <c r="F28" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1723,7 +1693,7 @@
         <v>41962</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="D29" s="52"/>
       <c r="E29" s="13"/>
@@ -1737,19 +1707,17 @@
         <v>41967</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>54</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D30" s="28"/>
       <c r="E30" s="60" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="I30" s="41">
         <v>5</v>
@@ -1761,13 +1729,13 @@
         <f t="shared" si="0"/>
         <v>41969</v>
       </c>
-      <c r="C31" s="68" t="s">
-        <v>93</v>
+      <c r="C31" s="67" t="s">
+        <v>81</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="58"/>
       <c r="F31" s="8" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1779,11 +1747,9 @@
         <v>41974</v>
       </c>
       <c r="C32" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>56</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D32" s="28"/>
       <c r="E32" s="38"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1792,16 +1758,16 @@
         <f t="shared" si="0"/>
         <v>41976</v>
       </c>
-      <c r="C33" s="65" t="s">
-        <v>59</v>
+      <c r="C33" s="64" t="s">
+        <v>48</v>
       </c>
       <c r="D33" s="55"/>
       <c r="E33" s="33" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F33" s="11"/>
       <c r="H33" s="41" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="I33" s="41">
         <v>10</v>
@@ -1815,15 +1781,15 @@
         <f t="shared" si="0"/>
         <v>41981</v>
       </c>
-      <c r="C34" s="64" t="s">
-        <v>61</v>
+      <c r="C34" s="63" t="s">
+        <v>50</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="27" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H34" s="40" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="I34" s="40">
         <v>20</v>
@@ -1839,7 +1805,7 @@
       <c r="D35" s="29"/>
       <c r="E35" s="17"/>
       <c r="H35" s="42" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I35" s="42">
         <v>10</v>
@@ -1854,7 +1820,7 @@
       </c>
       <c r="E36" s="46">
         <f ca="1">TODAY()</f>
-        <v>41918</v>
+        <v>41939</v>
       </c>
       <c r="I36" s="8">
         <f>SUM(I4:I35)</f>

</xml_diff>